<commit_message>
Quest localization, map button, map fixes, characters art
</commit_message>
<xml_diff>
--- a/Assets/Spreadsheet/Scripts/Map.xlsx
+++ b/Assets/Spreadsheet/Scripts/Map.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Map" sheetId="1" r:id="Rdf69a781d0a84403"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Map" sheetId="1" r:id="Rc0d7e938963545b3"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -13,9 +13,16 @@
     <x:t xml:space="preserve">Template</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">@hideUI QuestLogUI if:game_chapter==7
-@wait 1 if:game_chapter==7
-@set "game_chapter = -1" if:game_chapter==7
+    <x:t xml:space="preserve">
+@clearChoice ButtonArea
+@hideChars time:0
+@hideUI MapButtonUI time:0
+@showUI QuestLogUI if:game_chapter!=-1
+@if game_chapter==7
+@hideUI QuestLogUI
+@wait 1
+@set "game_chapter = -1"
+@endIf
 @hidePrinter 
 @choice  button:Map/Loc1 pos:-500,300 handler:ButtonArea goto:Loc1
 @choice  button:Map/Loc2 pos:700,125 handler:ButtonArea goto:Loc2

</xml_diff>